<commit_message>
fixed bugs in parent table
</commit_message>
<xml_diff>
--- a/manual/subsidiaries_to_search_hb_gmbh_auto.xlsx
+++ b/manual/subsidiaries_to_search_hb_gmbh_auto.xlsx
@@ -533,9 +533,13 @@
           <t>ARMCO Eisen G.m.b.H.</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Armco Eisengesellschaft</t>
+        </is>
+      </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>

</xml_diff>